<commit_message>
Adding More Metadata and EDA
</commit_message>
<xml_diff>
--- a/metadata/feature_descriptions.xlsx
+++ b/metadata/feature_descriptions.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{21CB1E6E-25F2-4AF0-A751-5FF13DF55614}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BE99010C-A198-4287-9FBB-E4B00222287F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="124">
   <si>
     <t xml:space="preserve">Variable </t>
   </si>
@@ -224,6 +224,174 @@
   </si>
   <si>
     <t>The number of beds in the facility</t>
+  </si>
+  <si>
+    <t>Feature Sub Categories</t>
+  </si>
+  <si>
+    <t>room-type</t>
+  </si>
+  <si>
+    <t>Entire home/apt    41310</t>
+  </si>
+  <si>
+    <t>Private room       30638</t>
+  </si>
+  <si>
+    <t>Shared room         2163</t>
+  </si>
+  <si>
+    <t>Apartment             49003</t>
+  </si>
+  <si>
+    <t>House                 16511</t>
+  </si>
+  <si>
+    <t>Condominium            2658</t>
+  </si>
+  <si>
+    <t>Townhouse              1692</t>
+  </si>
+  <si>
+    <t>Loft                   1244</t>
+  </si>
+  <si>
+    <t>Other                   607</t>
+  </si>
+  <si>
+    <t>Guesthouse              498</t>
+  </si>
+  <si>
+    <t>Bed &amp; Breakfast         462</t>
+  </si>
+  <si>
+    <t>Bungalow                366</t>
+  </si>
+  <si>
+    <t>Villa                   179</t>
+  </si>
+  <si>
+    <t>Dorm                    142</t>
+  </si>
+  <si>
+    <t>Guest suite             123</t>
+  </si>
+  <si>
+    <t>Camper/RV                94</t>
+  </si>
+  <si>
+    <t>Timeshare                77</t>
+  </si>
+  <si>
+    <t>Cabin                    72</t>
+  </si>
+  <si>
+    <t>In-law                   71</t>
+  </si>
+  <si>
+    <t>Hostel                   70</t>
+  </si>
+  <si>
+    <t>Boutique hotel           69</t>
+  </si>
+  <si>
+    <t>Boat                     65</t>
+  </si>
+  <si>
+    <t>Serviced apartment       21</t>
+  </si>
+  <si>
+    <t>Tent                     18</t>
+  </si>
+  <si>
+    <t>Castle                   13</t>
+  </si>
+  <si>
+    <t>Vacation home            11</t>
+  </si>
+  <si>
+    <t>Yurt                      9</t>
+  </si>
+  <si>
+    <t>Hut                       8</t>
+  </si>
+  <si>
+    <t>Treehouse                 7</t>
+  </si>
+  <si>
+    <t>Chalet                    6</t>
+  </si>
+  <si>
+    <t>Earth House               4</t>
+  </si>
+  <si>
+    <t>Tipi                      3</t>
+  </si>
+  <si>
+    <t>Cave                      2</t>
+  </si>
+  <si>
+    <t>Train                     2</t>
+  </si>
+  <si>
+    <t>Casa particular           1</t>
+  </si>
+  <si>
+    <t>Lighthouse                1</t>
+  </si>
+  <si>
+    <t>Parking Space             1</t>
+  </si>
+  <si>
+    <t>Island                    1</t>
+  </si>
+  <si>
+    <t>Real Bed         72028</t>
+  </si>
+  <si>
+    <t>Futon              753</t>
+  </si>
+  <si>
+    <t>Pull-out Sofa      585</t>
+  </si>
+  <si>
+    <t>Airbed             477</t>
+  </si>
+  <si>
+    <t>Couch              268</t>
+  </si>
+  <si>
+    <t>strict             32374</t>
+  </si>
+  <si>
+    <t>flexible           22545</t>
+  </si>
+  <si>
+    <t>moderate           19063</t>
+  </si>
+  <si>
+    <t>super_strict_30      112</t>
+  </si>
+  <si>
+    <t>super_strict_60       17</t>
+  </si>
+  <si>
+    <t>NYC        32349</t>
+  </si>
+  <si>
+    <t>LA         22453</t>
+  </si>
+  <si>
+    <t>SF          6434</t>
+  </si>
+  <si>
+    <t>DC          5688</t>
+  </si>
+  <si>
+    <t>Chicago     3719</t>
+  </si>
+  <si>
+    <t>Boston      3468</t>
   </si>
 </sst>
 </file>
@@ -560,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F33"/>
+  <dimension ref="B2:F95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42:E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1118,6 +1286,309 @@
         <v>131</v>
       </c>
     </row>
+    <row r="36" spans="2:6">
+      <c r="B36" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="B38" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="2:6">
+      <c r="C39" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6">
+      <c r="C40" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6">
+      <c r="C41" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6">
+      <c r="C42" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="2:6">
+      <c r="C43" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="2:6">
+      <c r="C44" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="2:6">
+      <c r="C45" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6">
+      <c r="C46" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6">
+      <c r="C47" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6">
+      <c r="C48" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3">
+      <c r="C49" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3">
+      <c r="C50" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3">
+      <c r="C51" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3">
+      <c r="C52" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3">
+      <c r="C53" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3">
+      <c r="C54" s="2" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="55" spans="3:3">
+      <c r="C55" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="56" spans="3:3">
+      <c r="C56" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="57" spans="3:3">
+      <c r="C57" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="58" spans="3:3">
+      <c r="C58" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3">
+      <c r="C59" s="2" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="60" spans="3:3">
+      <c r="C60" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="61" spans="3:3">
+      <c r="C61" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="62" spans="3:3">
+      <c r="C62" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="63" spans="3:3">
+      <c r="C63" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="64" spans="3:3">
+      <c r="C64" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3">
+      <c r="C65" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3">
+      <c r="C66" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3">
+      <c r="C67" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3">
+      <c r="C68" s="2" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3">
+      <c r="C69" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3">
+      <c r="C70" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3">
+      <c r="C71" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3">
+      <c r="C72" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="73" spans="2:3">
+      <c r="B73" s="2"/>
+    </row>
+    <row r="74" spans="2:3">
+      <c r="B74" t="s">
+        <v>69</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="75" spans="2:3">
+      <c r="C75" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="76" spans="2:3">
+      <c r="C76" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3">
+      <c r="B77" s="2"/>
+    </row>
+    <row r="78" spans="2:3">
+      <c r="B78" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C78" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="79" spans="2:3">
+      <c r="C79" s="2" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="80" spans="2:3">
+      <c r="C80" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="81" spans="2:3">
+      <c r="C81" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3">
+      <c r="C82" s="2" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3">
+      <c r="B83" s="2"/>
+    </row>
+    <row r="84" spans="2:3">
+      <c r="B84" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="85" spans="2:3">
+      <c r="C85" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="86" spans="2:3">
+      <c r="C86" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="87" spans="2:3">
+      <c r="C87" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3">
+      <c r="C88" s="2" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3">
+      <c r="B90" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C90" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="91" spans="2:3">
+      <c r="C91" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3">
+      <c r="C92" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3">
+      <c r="C93" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="94" spans="2:3">
+      <c r="C94" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3">
+      <c r="C95" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Feature Descriptions in the file
</commit_message>
<xml_diff>
--- a/metadata/feature_descriptions.xlsx
+++ b/metadata/feature_descriptions.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BE99010C-A198-4287-9FBB-E4B00222287F}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9AF4D28C-B753-4145-B69F-3BB98DD35FF8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="131">
   <si>
     <t xml:space="preserve">Variable </t>
   </si>
@@ -220,9 +220,6 @@
     <t>Zip Code of the Facility.</t>
   </si>
   <si>
-    <t>The bumber of bedrooms available.</t>
-  </si>
-  <si>
     <t>The number of beds in the facility</t>
   </si>
   <si>
@@ -392,6 +389,30 @@
   </si>
   <si>
     <t>Boston      3468</t>
+  </si>
+  <si>
+    <t>Used to Explain</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>Host</t>
+  </si>
+  <si>
+    <t>Property, Host</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>Property, host</t>
+  </si>
+  <si>
+    <t>Customers</t>
+  </si>
+  <si>
+    <t>The number of bedrooms available.</t>
   </si>
 </sst>
 </file>
@@ -728,10 +749,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F95"/>
+  <dimension ref="B2:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="E42" sqref="E42:E44"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -740,14 +761,15 @@
     <col min="2" max="2" width="14.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.109375" customWidth="1"/>
     <col min="4" max="4" width="70.88671875" customWidth="1"/>
+    <col min="7" max="7" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:7">
       <c r="B2" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:7">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -763,8 +785,11 @@
       <c r="F4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="2:6">
+      <c r="G4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
@@ -781,8 +806,11 @@
         <f>74111 - E5</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:6">
+      <c r="G5" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
       <c r="B6" s="2" t="s">
         <v>5</v>
       </c>
@@ -799,8 +827,11 @@
         <f t="shared" ref="F6:F33" si="0">74111 - E6</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="2:6">
+      <c r="G6" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7">
       <c r="B7" s="2" t="s">
         <v>6</v>
       </c>
@@ -817,8 +848,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="2:6">
+      <c r="G7" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7">
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
@@ -835,8 +869,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:6">
+      <c r="G8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7">
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
@@ -853,8 +890,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:6">
+      <c r="G9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7">
       <c r="B10" s="2" t="s">
         <v>9</v>
       </c>
@@ -871,8 +911,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="2:6">
+      <c r="G10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
       <c r="B11" s="2" t="s">
         <v>10</v>
       </c>
@@ -889,8 +932,11 @@
         <f t="shared" si="0"/>
         <v>200</v>
       </c>
-    </row>
-    <row r="12" spans="2:6">
+      <c r="G11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
       <c r="B12" s="2" t="s">
         <v>11</v>
       </c>
@@ -907,8 +953,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="2:6">
+      <c r="G12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7">
       <c r="B13" s="2" t="s">
         <v>12</v>
       </c>
@@ -925,8 +974,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="2:6">
+      <c r="G13" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7">
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
@@ -943,8 +995,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="2:6">
+      <c r="G14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
       <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
@@ -961,8 +1016,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="2:6">
+      <c r="G15" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7">
       <c r="B16" s="2" t="s">
         <v>15</v>
       </c>
@@ -979,8 +1037,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="2:6">
+      <c r="G16" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
       <c r="B17" s="2" t="s">
         <v>16</v>
       </c>
@@ -997,8 +1058,11 @@
         <f t="shared" si="0"/>
         <v>15864</v>
       </c>
-    </row>
-    <row r="18" spans="2:6">
+      <c r="G17" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
       <c r="B18" s="2" t="s">
         <v>17</v>
       </c>
@@ -1015,8 +1079,11 @@
         <f t="shared" si="0"/>
         <v>188</v>
       </c>
-    </row>
-    <row r="19" spans="2:6">
+      <c r="G18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7">
       <c r="B19" s="2" t="s">
         <v>18</v>
       </c>
@@ -1033,8 +1100,11 @@
         <f t="shared" si="0"/>
         <v>188</v>
       </c>
-    </row>
-    <row r="20" spans="2:6">
+      <c r="G19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
       <c r="B20" s="2" t="s">
         <v>19</v>
       </c>
@@ -1051,8 +1121,11 @@
         <f t="shared" si="0"/>
         <v>18299</v>
       </c>
-    </row>
-    <row r="21" spans="2:6">
+      <c r="G20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
       <c r="B21" s="2" t="s">
         <v>20</v>
       </c>
@@ -1069,8 +1142,11 @@
         <f t="shared" si="0"/>
         <v>188</v>
       </c>
-    </row>
-    <row r="22" spans="2:6">
+      <c r="G21" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
       <c r="B22" s="2" t="s">
         <v>21</v>
       </c>
@@ -1087,8 +1163,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="2:6">
+      <c r="G22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
       <c r="B23" s="2" t="s">
         <v>22</v>
       </c>
@@ -1105,8 +1184,11 @@
         <f t="shared" si="0"/>
         <v>15827</v>
       </c>
-    </row>
-    <row r="24" spans="2:6">
+      <c r="G23" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7">
       <c r="B24" s="2" t="s">
         <v>23</v>
       </c>
@@ -1123,8 +1205,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="2:6">
+      <c r="G24" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7">
       <c r="B25" s="2" t="s">
         <v>24</v>
       </c>
@@ -1141,8 +1226,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="2:6">
+      <c r="G25" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7">
       <c r="B26" s="2" t="s">
         <v>25</v>
       </c>
@@ -1159,8 +1247,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="2:6">
+      <c r="G26" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7">
       <c r="B27" s="2" t="s">
         <v>26</v>
       </c>
@@ -1177,8 +1268,11 @@
         <f t="shared" si="0"/>
         <v>6872</v>
       </c>
-    </row>
-    <row r="28" spans="2:6">
+      <c r="G27" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7">
       <c r="B28" s="2" t="s">
         <v>27</v>
       </c>
@@ -1195,8 +1289,11 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="2:6">
+      <c r="G28" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7">
       <c r="B29" s="2" t="s">
         <v>28</v>
       </c>
@@ -1213,8 +1310,11 @@
         <f t="shared" si="0"/>
         <v>16722</v>
       </c>
-    </row>
-    <row r="30" spans="2:6">
+      <c r="G29" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7">
       <c r="B30" s="2" t="s">
         <v>29</v>
       </c>
@@ -1231,8 +1331,11 @@
         <f t="shared" si="0"/>
         <v>8216</v>
       </c>
-    </row>
-    <row r="31" spans="2:6">
+      <c r="G30" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7">
       <c r="B31" s="2" t="s">
         <v>30</v>
       </c>
@@ -1249,8 +1352,11 @@
         <f t="shared" si="0"/>
         <v>966</v>
       </c>
-    </row>
-    <row r="32" spans="2:6">
+      <c r="G31" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7">
       <c r="B32" s="2" t="s">
         <v>31</v>
       </c>
@@ -1258,7 +1364,7 @@
         <v>35</v>
       </c>
       <c r="D32" t="s">
-        <v>66</v>
+        <v>130</v>
       </c>
       <c r="E32">
         <v>74020</v>
@@ -1267,8 +1373,11 @@
         <f t="shared" si="0"/>
         <v>91</v>
       </c>
-    </row>
-    <row r="33" spans="2:6">
+      <c r="G32" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7">
       <c r="B33" s="2" t="s">
         <v>32</v>
       </c>
@@ -1276,7 +1385,7 @@
         <v>35</v>
       </c>
       <c r="D33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E33">
         <v>73980</v>
@@ -1285,192 +1394,195 @@
         <f t="shared" si="0"/>
         <v>131</v>
       </c>
-    </row>
-    <row r="36" spans="2:6">
+      <c r="G33" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7">
       <c r="B36" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="2:6">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7">
       <c r="B38" s="2" t="s">
         <v>6</v>
       </c>
       <c r="C38" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E38" s="2"/>
+    </row>
+    <row r="39" spans="2:7">
+      <c r="C39" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E38" s="2"/>
-    </row>
-    <row r="39" spans="2:6">
-      <c r="C39" s="2" t="s">
+    </row>
+    <row r="40" spans="2:7">
+      <c r="C40" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="2:6">
-      <c r="C40" s="2" t="s">
+    <row r="41" spans="2:7">
+      <c r="C41" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="2:6">
-      <c r="C41" s="2" t="s">
+    <row r="42" spans="2:7">
+      <c r="C42" s="2" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="42" spans="2:6">
-      <c r="C42" s="2" t="s">
+      <c r="E42" s="2"/>
+    </row>
+    <row r="43" spans="2:7">
+      <c r="C43" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E42" s="2"/>
-    </row>
-    <row r="43" spans="2:6">
-      <c r="C43" s="2" t="s">
+      <c r="E43" s="2"/>
+    </row>
+    <row r="44" spans="2:7">
+      <c r="C44" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E43" s="2"/>
-    </row>
-    <row r="44" spans="2:6">
-      <c r="C44" s="2" t="s">
+      <c r="E44" s="2"/>
+    </row>
+    <row r="45" spans="2:7">
+      <c r="C45" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E44" s="2"/>
-    </row>
-    <row r="45" spans="2:6">
-      <c r="C45" s="2" t="s">
+    </row>
+    <row r="46" spans="2:7">
+      <c r="C46" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="46" spans="2:6">
-      <c r="C46" s="2" t="s">
+    <row r="47" spans="2:7">
+      <c r="C47" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="47" spans="2:6">
-      <c r="C47" s="2" t="s">
+    <row r="48" spans="2:7">
+      <c r="C48" s="2" t="s">
         <v>82</v>
-      </c>
-    </row>
-    <row r="48" spans="2:6">
-      <c r="C48" s="2" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="49" spans="3:3">
       <c r="C49" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="3:3">
       <c r="C50" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="51" spans="3:3">
       <c r="C51" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="52" spans="3:3">
       <c r="C52" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="53" spans="3:3">
       <c r="C53" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="54" spans="3:3">
       <c r="C54" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="55" spans="3:3">
       <c r="C55" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="3:3">
       <c r="C56" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="57" spans="3:3">
       <c r="C57" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="58" spans="3:3">
       <c r="C58" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="59" spans="3:3">
       <c r="C59" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="60" spans="3:3">
       <c r="C60" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="61" spans="3:3">
       <c r="C61" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="62" spans="3:3">
       <c r="C62" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="63" spans="3:3">
       <c r="C63" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="64" spans="3:3">
       <c r="C64" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="65" spans="2:3">
       <c r="C65" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="66" spans="2:3">
       <c r="C66" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="67" spans="2:3">
       <c r="C67" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="68" spans="2:3">
       <c r="C68" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="69" spans="2:3">
       <c r="C69" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="70" spans="2:3">
       <c r="C70" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="71" spans="2:3">
       <c r="C71" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="72" spans="2:3">
       <c r="C72" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="73" spans="2:3">
@@ -1478,20 +1590,20 @@
     </row>
     <row r="74" spans="2:3">
       <c r="B74" t="s">
+        <v>68</v>
+      </c>
+      <c r="C74" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="75" spans="2:3">
       <c r="C75" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="76" spans="2:3">
       <c r="C76" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="77" spans="2:3">
@@ -1502,27 +1614,27 @@
         <v>11</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="79" spans="2:3">
       <c r="C79" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="80" spans="2:3">
       <c r="C80" s="2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="81" spans="2:3">
       <c r="C81" s="2" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="82" spans="2:3">
       <c r="C82" s="2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="83" spans="2:3">
@@ -1533,27 +1645,27 @@
         <v>12</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="85" spans="2:3">
       <c r="C85" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="86" spans="2:3">
       <c r="C86" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="87" spans="2:3">
       <c r="C87" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="88" spans="2:3">
       <c r="C88" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="90" spans="2:3">
@@ -1561,32 +1673,32 @@
         <v>14</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="91" spans="2:3">
       <c r="C91" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="92" spans="2:3">
       <c r="C92" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="93" spans="2:3">
       <c r="C93" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="94" spans="2:3">
       <c r="C94" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="95" spans="2:3">
       <c r="C95" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated the Source Files + Integration
Updated the Source Files and Integrated a portion of the changes
</commit_message>
<xml_diff>
--- a/metadata/feature_descriptions.xlsx
+++ b/metadata/feature_descriptions.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9AF4D28C-B753-4145-B69F-3BB98DD35FF8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{FE6087B8-AADB-4C2F-A469-BBC586B5482D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="134">
   <si>
     <t xml:space="preserve">Variable </t>
   </si>
@@ -413,6 +413,15 @@
   </si>
   <si>
     <t>The number of bedrooms available.</t>
+  </si>
+  <si>
+    <t>Listing</t>
+  </si>
+  <si>
+    <t>Listing, Property</t>
+  </si>
+  <si>
+    <t>Listing, Property, host</t>
   </si>
 </sst>
 </file>
@@ -751,8 +760,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:G95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:XFD18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -807,7 +816,7 @@
         <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
     </row>
     <row r="6" spans="2:7">
@@ -828,7 +837,7 @@
         <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
     </row>
     <row r="7" spans="2:7">
@@ -891,7 +900,7 @@
         <v>0</v>
       </c>
       <c r="G9" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="2:7">
@@ -975,7 +984,7 @@
         <v>0</v>
       </c>
       <c r="G13" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="2:7">
@@ -996,7 +1005,7 @@
         <v>0</v>
       </c>
       <c r="G14" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="2:7">
@@ -1038,10 +1047,10 @@
         <v>0</v>
       </c>
       <c r="G16" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="16.8" customHeight="1">
       <c r="B17" s="2" t="s">
         <v>16</v>
       </c>
@@ -1164,7 +1173,7 @@
         <v>0</v>
       </c>
       <c r="G22" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="2:7">
@@ -1332,7 +1341,7 @@
         <v>8216</v>
       </c>
       <c r="G30" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="2:7">

</xml_diff>